<commit_message>
Modified   PositionBasedDynamics/.gitignore Modified   doc/fluid_painter.xlsx Modified   doc/基于物理的流体渲染——从理论到实践.md Added      doc/image/rigidcontactconstraint-sdf.png Added      doc/image/rigidcontactconstraint-sparse-sdf.png
</commit_message>
<xml_diff>
--- a/doc/fluid_painter.xlsx
+++ b/doc/fluid_painter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\private\UnityFluid\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F800CF60-0CB1-4BE6-A4B6-68ED1FFE55AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FA0817-C040-4554-BBEE-E6E5ED2465BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{89DEF0B8-0BD3-480E-A49C-887E929FBB58}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -604,8 +605,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="225895" cy="242118"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="18" name="文本框 17">
@@ -647,6 +648,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -676,7 +678,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="18" name="文本框 17">
@@ -806,6 +808,2451 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="椭圆 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{426534D7-E6B4-42B5-A310-EC384A449E23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2121529">
+          <a:off x="10201275" y="828675"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>200026</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="直接箭头连接符 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B927208-28D2-41D4-978C-8DD082EEEFE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11315700" y="2543175"/>
+          <a:ext cx="276225" cy="257176"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>361951</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="椭圆 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7FB8121-1D6B-41E4-A3F0-F6FCA83C8A66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2121529">
+          <a:off x="10401300" y="1123950"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>276226</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="椭圆 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{770872C1-13D9-41EF-82AB-09C7A2D2542F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2121529">
+          <a:off x="10601325" y="1409700"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>238126</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="椭圆 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACB35417-6873-4191-8FAD-EE90F701E0A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7762875" y="1743075"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>238126</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="椭圆 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{464983FE-942B-48C6-823F-B5BE1605300D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2121529">
+          <a:off x="10496550" y="628650"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="椭圆 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E09E40E-39B1-4DA3-A275-4AA3D79358AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2121529">
+          <a:off x="10687050" y="923925"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="椭圆 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{497775EF-0974-4221-A0D1-E840CB84EAD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2121529">
+          <a:off x="10887075" y="1219200"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="椭圆 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA56F4CE-E9DE-4100-A227-9357F8402E47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2121529">
+          <a:off x="11087100" y="1514475"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="椭圆 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBDD5FDA-63FF-45D8-AD69-49A8A85FD516}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11153775" y="2990850"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="椭圆 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9320607-0429-4962-9F3A-E334E785096F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11153775" y="3362325"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="椭圆 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14948E6A-A621-4A0A-A214-0CF9C230BF4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11153775" y="2619374"/>
+          <a:ext cx="361950" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="椭圆 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92C47095-1981-4400-AEB4-F68828C8E64C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10782300" y="2628900"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="椭圆 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA1C4B8A-C299-4070-BE22-24C2A84F4910}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10782300" y="3000375"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="椭圆 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE06CFDF-A111-47AE-BED4-962223CDA992}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10782300" y="3362325"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>350022</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>219640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>326331</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171191</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="矩形 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BB146A9-DB6D-453F-B43A-C7BA2E9A183F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14923272" y="2835352"/>
+          <a:ext cx="723655" cy="1446243"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="椭圆 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0F12203-7012-406D-A139-210B6D62E73B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10944225" y="2362200"/>
+          <a:ext cx="361950" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114302</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="椭圆 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6DC4E56-7992-493E-8252-1C0B08D711D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10944225" y="2733676"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>123827</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="椭圆 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B075B74F-7807-4898-84B8-E8C20F0BF6EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10572750" y="2371726"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123827</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="椭圆 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E431A028-FE7B-4300-8EB2-B87D427B9984}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10572750" y="2743201"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="椭圆 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD5C5791-C1FE-4DF4-8BA8-3A6ADB4830CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15249525" y="2962275"/>
+          <a:ext cx="361950" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>361951</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>342902</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="椭圆 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA0647B7-B642-48E0-9B79-1B89F8ED6232}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15249525" y="3333751"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>361951</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>342902</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="椭圆 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCDC6786-F76F-4E66-9AC4-DE070ACB3B3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15249525" y="3705226"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>352427</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="椭圆 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A1454DC-D04A-4E57-9675-263C4E012E67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14878050" y="2971801"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>352427</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="椭圆 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D64952E-80CD-45AF-83D6-92CD557793BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14878050" y="3343276"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>361951</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>342902</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="椭圆 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE998CD9-9FE1-4B0E-8E73-D8828D0C627E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14878050" y="3705226"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="椭圆 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EECCA0E6-0D09-4FC9-BEA9-AE04B86693CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10944225" y="2009775"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="椭圆 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F806D1E-849F-4849-B852-B188752A0DBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10572750" y="2019300"/>
+          <a:ext cx="361950" cy="352426"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>361953</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="直接箭头连接符 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C4DE102-0446-4C09-AB69-12D2E6ABEEF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11134728" y="2543175"/>
+          <a:ext cx="409572" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>360044</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="箭头: 右 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5385C864-2EC9-45A3-98F3-66881456EAC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="10106025" y="2447925"/>
+          <a:ext cx="361950" cy="140969"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>295276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="箭头: 右 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A2E2257-4D10-4687-A8D6-F96474925347}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="8181687">
+          <a:off x="10248900" y="3267076"/>
+          <a:ext cx="361950" cy="140969"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>236219</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="箭头: 右 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FA76ABA-EC2A-47EE-A318-0154B04D426A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11630025" y="3067050"/>
+          <a:ext cx="361950" cy="140969"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>339970</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>330445</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="椭圆 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75A59510-2526-4C70-8CFF-54BE71A42E5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15660566" y="3160835"/>
+          <a:ext cx="364148" cy="373673"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="48000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="97000"/>
+                <a:lumOff val="3000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1108,8 +3555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9666C506-C06A-4B74-9994-EE4F9F570611}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AR11" sqref="AR11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>